<commit_message>
Fixed Template parameters bug added requirements
</commit_message>
<xml_diff>
--- a/Template Files/CutOut Size Check.xlsx
+++ b/Template Files/CutOut Size Check.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23929"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Greg\OneDrive - Queen's University\Work\Plan Checking tools\ElectronCutout\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Greg\OneDrive - Queen's University\Work\Plan Checking tools\ElectronCutout\Template Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B386609F-09D6-4979-8D1C-8CE56A4AC960}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03DB0DF5-B6AE-402D-961A-C0FF4D49C59E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="705" windowWidth="19440" windowHeight="15150" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CutOut Image" sheetId="5" r:id="rId1"/>
@@ -2784,13 +2784,13 @@
   <dimension ref="O1:Q28"/>
   <sheetViews>
     <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="X19" sqref="X19"/>
+      <selection activeCell="P1" sqref="P1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="15" max="15" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="10.28515625" style="16" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.7109375" style="16" customWidth="1"/>
     <col min="17" max="17" width="5.5703125" style="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2962,7 +2962,7 @@
   <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>